<commit_message>
completed assessment of week 1 evals.
</commit_message>
<xml_diff>
--- a/Function 6/evals.xlsx
+++ b/Function 6/evals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prithvi\Desktop\Imperial Course\Capstone-Project\Function 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA1B1A-F02A-4662-B5DA-108302266464}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA2AB07-ABB5-4EBA-81DF-52AFAFB9838D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Query Number</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>x5</t>
+  </si>
+  <si>
+    <t>x6</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O14"/>
+  <dimension ref="B2:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4:O4"/>
@@ -389,7 +392,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -415,69 +418,81 @@
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
-        <v>0.28513226139336401</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>4.0108999999999999E-2</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4">
-        <v>0.59778317071714704</v>
+        <v>0.64410999999999996</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="2">
-        <v>1</v>
+        <v>0.120268</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2">
-        <v>1</v>
+        <v>0.35586299999999998</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2">
-        <v>-0.82197116627998901</v>
+        <v>0.87413600000000002</v>
       </c>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="2">
+        <v>1.39427779979913</v>
+      </c>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
-        <v>0.35840106518858</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>0.28961338659042302</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
-        <v>1</v>
+        <v>6.13308944438598E-2</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
+        <v>0.34585898347106497</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2">
         <v>1</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -491,7 +506,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -505,7 +520,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -519,7 +534,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -533,7 +548,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -547,7 +562,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -561,7 +576,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -575,7 +590,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -589,7 +604,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -603,7 +618,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -618,8 +633,8 @@
       <c r="M14" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="N2:O2"/>
+  <mergeCells count="64">
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="J2:K2"/>
@@ -628,6 +643,9 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>

</xml_diff>

<commit_message>
week 2 evals sent.
</commit_message>
<xml_diff>
--- a/Function 6/evals.xlsx
+++ b/Function 6/evals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prithvi\Desktop\Imperial Course\Capstone-Project\Function 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA2AB07-ABB5-4EBA-81DF-52AFAFB9838D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CC4761-A00E-4D88-870B-3067B35F12D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Query Number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>x5</t>
-  </si>
-  <si>
-    <t>x6</t>
   </si>
 </sst>
 </file>
@@ -95,10 +92,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -384,274 +381,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q14"/>
+  <dimension ref="B2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:O4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>0.28513226139336401</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>4.0108999999999999E-2</v>
-      </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="4">
-        <v>0.64410999999999996</v>
+        <v>0.59778317071714704</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="2">
-        <v>0.120268</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2">
-        <v>0.35586299999999998</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2">
-        <v>0.87413600000000002</v>
-      </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2">
-        <v>1.39427779979913</v>
-      </c>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3">
+        <v>-0.82197116627998901</v>
+      </c>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.35840106518858</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
-        <v>0.28961338659042302</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2">
-        <v>6.13308944438598E-2</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2">
-        <v>0.34585898347106497</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+  <mergeCells count="61">
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H9:I9"/>
@@ -664,40 +665,21 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>